<commit_message>
Add Azure Resource Graph assets to Asset Inventory (#2423)
</commit_message>
<xml_diff>
--- a/internal/inventory/cloud_assets.xlsx
+++ b/internal/inventory/cloud_assets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RAW list of all cloud services" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1072">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -2673,9 +2673,6 @@
   </si>
   <si>
     <t xml:space="preserve">AzureSQLServer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relational Database</t>
   </si>
   <si>
     <t xml:space="preserve">Azure SQL Server</t>
@@ -3896,7 +3893,7 @@
   <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="D5 D9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6080,10 +6077,10 @@
   </sheetPr>
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G88" activeCellId="0" sqref="G88"/>
+      <selection pane="bottomLeft" activeCell="G88" activeCellId="2" sqref="D5 D9 G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8311,7 +8308,7 @@
       <c r="D86" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="E86" s="0" t="s">
+      <c r="E86" s="1" t="s">
         <v>803</v>
       </c>
       <c r="F86" s="1" t="n">
@@ -8336,10 +8333,10 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="2" sqref="D5 D9 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8446,18 +8443,18 @@
         <v>87</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>813</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>814</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>418</v>
@@ -8469,15 +8466,15 @@
         <v>68</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>817</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>418</v>
@@ -8486,18 +8483,18 @@
         <v>87</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>821</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>449</v>
@@ -8509,7 +8506,7 @@
         <v>766</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>806</v>
@@ -8517,7 +8514,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>418</v>
@@ -8526,38 +8523,38 @@
         <v>87</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>813</v>
+        <v>444</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>826</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>418</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>683</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>830</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>418</v>
@@ -8569,15 +8566,15 @@
         <v>69</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>833</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>418</v>
@@ -8586,18 +8583,18 @@
         <v>87</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>836</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>418</v>
@@ -8609,15 +8606,15 @@
         <v>530</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>839</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>449</v>
@@ -8626,18 +8623,18 @@
         <v>450</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>843</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>418</v>
@@ -8646,18 +8643,18 @@
         <v>87</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>847</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>418</v>
@@ -8666,18 +8663,18 @@
         <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>850</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>418</v>
@@ -8686,18 +8683,18 @@
         <v>87</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>854</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>418</v>
@@ -8706,18 +8703,18 @@
         <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>858</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>418</v>
@@ -8726,18 +8723,18 @@
         <v>87</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>862</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>418</v>
@@ -8746,18 +8743,18 @@
         <v>651</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>866</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>418</v>
@@ -8766,18 +8763,18 @@
         <v>87</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>869</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>418</v>
@@ -8789,15 +8786,15 @@
         <v>652</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>872</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>418</v>
@@ -8806,18 +8803,18 @@
         <v>87</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>875</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>418</v>
@@ -8826,38 +8823,38 @@
         <v>68</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>879</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>418</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>683</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>882</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>418</v>
@@ -8866,18 +8863,18 @@
         <v>87</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>885</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>418</v>
@@ -8886,18 +8883,18 @@
         <v>68</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>888</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>418</v>
@@ -8909,15 +8906,15 @@
         <v>69</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>891</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>418</v>
@@ -8926,18 +8923,18 @@
         <v>87</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>894</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>418</v>
@@ -8946,18 +8943,18 @@
         <v>651</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>898</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>418</v>
@@ -8966,18 +8963,18 @@
         <v>87</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>901</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>418</v>
@@ -8989,15 +8986,15 @@
         <v>162</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>904</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>418</v>
@@ -9006,18 +9003,18 @@
         <v>428</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>908</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>418</v>
@@ -9026,18 +9023,18 @@
         <v>87</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>911</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>418</v>
@@ -9046,18 +9043,18 @@
         <v>87</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>914</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>418</v>
@@ -9066,18 +9063,18 @@
         <v>87</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E36" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>917</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>418</v>
@@ -9086,18 +9083,18 @@
         <v>87</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>920</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>418</v>
@@ -9106,18 +9103,18 @@
         <v>87</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E38" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>923</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>418</v>
@@ -9126,18 +9123,18 @@
         <v>87</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E39" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>926</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>418</v>
@@ -9149,15 +9146,15 @@
         <v>674</v>
       </c>
       <c r="E40" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>929</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>418</v>
@@ -9169,15 +9166,15 @@
         <v>674</v>
       </c>
       <c r="E41" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>932</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>418</v>
@@ -9189,141 +9186,141 @@
         <v>642</v>
       </c>
       <c r="E42" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>935</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>478</v>
       </c>
       <c r="E43" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>939</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>757</v>
       </c>
       <c r="E44" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="H44" s="5" t="s">
         <v>942</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C45" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>947</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>950</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>950</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="H46" s="5" t="s">
         <v>951</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>451</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="I48" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="J48" s="5" t="s">
         <v>961</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -9332,38 +9329,38 @@
         <v>488</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="H49" s="5" t="s">
         <v>965</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>418</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>968</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>969</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>418</v>
@@ -9372,18 +9369,18 @@
         <v>462</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="H51" s="5" t="s">
         <v>973</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>418</v>
@@ -9398,7 +9395,7 @@
         <v>32</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -9422,7 +9419,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="2" sqref="D5 D9 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9463,7 +9460,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>418</v>
@@ -9475,15 +9472,15 @@
         <v>489</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>978</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>418</v>
@@ -9495,15 +9492,15 @@
         <v>423</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>981</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>418</v>
@@ -9515,15 +9512,15 @@
         <v>434</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>418</v>
@@ -9535,15 +9532,15 @@
         <v>525</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>986</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>987</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>418</v>
@@ -9555,15 +9552,15 @@
         <v>429</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>990</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>418</v>
@@ -9575,15 +9572,15 @@
         <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>993</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>418</v>
@@ -9595,15 +9592,15 @@
         <v>457</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>996</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>418</v>
@@ -9615,15 +9612,15 @@
         <v>530</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>418</v>
@@ -9635,15 +9632,15 @@
         <v>489</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>1002</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>418</v>
@@ -9652,18 +9649,18 @@
         <v>428</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1006</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>418</v>
@@ -9672,18 +9669,18 @@
         <v>488</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>418</v>
@@ -9692,18 +9689,18 @@
         <v>428</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>1014</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>418</v>
@@ -9715,15 +9712,15 @@
         <v>612</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>1017</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>1018</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>418</v>
@@ -9735,15 +9732,15 @@
         <v>493</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>1020</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>418</v>
@@ -9752,18 +9749,18 @@
         <v>428</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>1023</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>418</v>
@@ -9775,15 +9772,15 @@
         <v>429</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>1026</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>418</v>
@@ -9795,115 +9792,115 @@
         <v>530</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>1029</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>488</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>1032</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>1034</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>1038</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>1042</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>468</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>1045</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>452</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>1048</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>418</v>
@@ -9912,18 +9909,18 @@
         <v>462</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E24" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>1051</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>418</v>
@@ -9935,15 +9932,15 @@
         <v>462</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>1054</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>418</v>
@@ -9952,13 +9949,13 @@
         <v>428</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>1057</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>1058</v>
       </c>
     </row>
   </sheetData>
@@ -9982,7 +9979,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="2" sqref="D5 D9 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10041,7 +10038,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -10051,10 +10048,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>1060</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>1061</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -10077,7 +10074,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -10087,10 +10084,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>1063</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1064</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -10113,7 +10110,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -10123,10 +10120,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>1066</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>1067</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -10149,7 +10146,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -10159,10 +10156,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>1069</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>1070</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -10185,7 +10182,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -10215,7 +10212,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>

</xml_diff>